<commit_message>
adicionado consulta e geração dados
</commit_message>
<xml_diff>
--- a/mmv.xlsx
+++ b/mmv.xlsx
@@ -77,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -127,6 +127,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>